<commit_message>
suppression de la balise meta keyword
</commit_message>
<xml_diff>
--- a/Audit.xlsx
+++ b/Audit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bacarifayad/Desktop/Openclasseroom/Projet 4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B182470B-EB95-BC49-94F7-51A6BD094C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE686603-214C-6E4C-930A-D5736E5B540B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -663,7 +663,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -751,7 +751,7 @@
         <v>77</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>82</v>
@@ -771,7 +771,7 @@
         <v>77</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>82</v>
@@ -791,7 +791,7 @@
         <v>77</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>83</v>
@@ -811,7 +811,7 @@
         <v>77</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>83</v>
@@ -831,7 +831,7 @@
         <v>77</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>84</v>
@@ -1111,7 +1111,7 @@
         <v>67</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F21" s="7" t="s">
         <v>97</v>
@@ -1151,7 +1151,7 @@
         <v>65</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>99</v>
@@ -1171,7 +1171,7 @@
         <v>64</v>
       </c>
       <c r="E24" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F24" s="7" t="s">
         <v>100</v>

</xml_diff>

<commit_message>
suprétion des des images text
</commit_message>
<xml_diff>
--- a/Audit.xlsx
+++ b/Audit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bacarifayad/Desktop/Openclasseroom/Projet 4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B335BCEE-FA33-B340-957B-E089719B8450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD73E57A-08FE-9D4C-B934-284850A28E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -361,7 +361,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -398,6 +398,12 @@
       <color theme="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -433,7 +439,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -447,6 +453,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -666,7 +673,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -994,7 +1001,7 @@
         <v>72</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>62</v>
+        <v>107</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>92</v>
@@ -1273,8 +1280,8 @@
       <c r="D29" t="s">
         <v>78</v>
       </c>
-      <c r="E29" t="s">
-        <v>62</v>
+      <c r="E29" s="9" t="s">
+        <v>107</v>
       </c>
       <c r="F29" s="7" t="s">
         <v>106</v>

</xml_diff>

<commit_message>
ajout d'une meta description
</commit_message>
<xml_diff>
--- a/Audit.xlsx
+++ b/Audit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bacarifayad/Desktop/Openclasseroom/Projet 4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AFEEB55-68B1-DC46-A68D-C48614CE14C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B17A9E-E79D-D341-B2D5-16A4287D8145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="5720" windowWidth="28800" windowHeight="16180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="107">
   <si>
     <t>Catégorie</t>
   </si>
@@ -217,9 +217,6 @@
   </si>
   <si>
     <t>Element non autorisé dans le HTML.</t>
-  </si>
-  <si>
-    <t>Oui</t>
   </si>
   <si>
     <t>Non</t>
@@ -673,7 +670,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -738,13 +735,13 @@
         <v>48</v>
       </c>
       <c r="D2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -758,13 +755,13 @@
         <v>49</v>
       </c>
       <c r="D3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -778,13 +775,13 @@
         <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -798,13 +795,13 @@
         <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -818,13 +815,13 @@
         <v>61</v>
       </c>
       <c r="D6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -838,13 +835,13 @@
         <v>60</v>
       </c>
       <c r="D7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -858,13 +855,13 @@
         <v>46</v>
       </c>
       <c r="D8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -878,13 +875,13 @@
         <v>45</v>
       </c>
       <c r="D9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -898,13 +895,13 @@
         <v>44</v>
       </c>
       <c r="D10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -918,13 +915,13 @@
         <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -938,13 +935,13 @@
         <v>43</v>
       </c>
       <c r="D12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -958,13 +955,13 @@
         <v>41</v>
       </c>
       <c r="D13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -978,13 +975,13 @@
         <v>40</v>
       </c>
       <c r="D14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -998,13 +995,13 @@
         <v>39</v>
       </c>
       <c r="D15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1018,13 +1015,13 @@
         <v>38</v>
       </c>
       <c r="D16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1038,13 +1035,13 @@
         <v>35</v>
       </c>
       <c r="D17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1058,13 +1055,13 @@
         <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1078,13 +1075,13 @@
         <v>37</v>
       </c>
       <c r="D19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1098,13 +1095,13 @@
         <v>36</v>
       </c>
       <c r="D20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1118,13 +1115,13 @@
         <v>50</v>
       </c>
       <c r="D21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1138,13 +1135,13 @@
         <v>52</v>
       </c>
       <c r="D22" t="s">
-        <v>66</v>
-      </c>
-      <c r="E22" t="s">
-        <v>62</v>
+        <v>65</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>106</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1158,13 +1155,13 @@
         <v>53</v>
       </c>
       <c r="D23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1178,13 +1175,13 @@
         <v>54</v>
       </c>
       <c r="D24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1198,13 +1195,13 @@
         <v>55</v>
       </c>
       <c r="D25" t="s">
+        <v>100</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" s="7" t="s">
         <v>101</v>
-      </c>
-      <c r="E25" t="s">
-        <v>62</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1218,13 +1215,13 @@
         <v>56</v>
       </c>
       <c r="D26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1238,13 +1235,13 @@
         <v>57</v>
       </c>
       <c r="D27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1258,13 +1255,13 @@
         <v>58</v>
       </c>
       <c r="D28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1278,13 +1275,13 @@
         <v>59</v>
       </c>
       <c r="D29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
changement de coulor pour l'obtimation
</commit_message>
<xml_diff>
--- a/Audit.xlsx
+++ b/Audit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bacarifayad/Desktop/Openclasseroom/Projet 4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B17A9E-E79D-D341-B2D5-16A4287D8145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D93909F-7459-2A49-9875-B2FA5B5ECF4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5720" windowWidth="28800" windowHeight="16180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="540" windowWidth="28800" windowHeight="16180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="107">
   <si>
     <t>Catégorie</t>
   </si>
@@ -670,7 +670,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1285,6 +1285,9 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>33</v>
+      </c>
       <c r="F30" s="7"/>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>